<commit_message>
Updated money actions to not take place on DEBUG constant set Updated Table Properties.xlsx
</commit_message>
<xml_diff>
--- a/branches/ ultimate-business-mod/UltimateBusinessMod/Development Data/Database/Table Properties.xlsx
+++ b/branches/ ultimate-business-mod/UltimateBusinessMod/Development Data/Database/Table Properties.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Field Explanation" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
   <si>
     <t>Grotti</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Used as 'bulk storage' for the boolean variables [Ownable][Owned][ContextMission]</t>
   </si>
   <si>
-    <t>Stored as a single integer value</t>
-  </si>
-  <si>
     <t>Eg.: 101</t>
   </si>
   <si>
@@ -138,12 +135,6 @@
     <t>Unsed when flag is already true</t>
   </si>
   <si>
-    <t>Refer to page Types for more info</t>
-  </si>
-  <si>
-    <t>Integer</t>
-  </si>
-  <si>
     <t>Showroom</t>
   </si>
   <si>
@@ -171,28 +162,55 @@
     <t>ID</t>
   </si>
   <si>
-    <t>StaffIncome</t>
-  </si>
-  <si>
-    <t>N/D</t>
-  </si>
-  <si>
-    <t>0/0</t>
-  </si>
-  <si>
-    <t>500/1000</t>
-  </si>
-  <si>
-    <t>150/250</t>
-  </si>
-  <si>
-    <t>50/100</t>
-  </si>
-  <si>
-    <t>250/500</t>
-  </si>
-  <si>
-    <t>CREATE TABLE [Properties] ([ID] INTEGER  NOT NULL PRIMARY KEY AUTOINCREMENT,[Name] VARCHAR(30)  UNIQUE NOT NULL,[Location] VARCHAR(150)  UNIQUE NOT NULL,[Flags] VARCHAR(3)  NOT NULL,[Staff] INTEGER DEFAULT '0' NOT NULL,[StaffCap] INTEGER DEFAULT '10' NOT NULL,[Cost] INTEGER  NOT NULL, [TypeID] INTEGER  NOT NULL)</t>
+    <t>IncomeMin</t>
+  </si>
+  <si>
+    <t>IncomeMax</t>
+  </si>
+  <si>
+    <t>StaffSal</t>
+  </si>
+  <si>
+    <t>StaffPay</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>CREATE TABLE [Properties] ([ID] INTEGER  PRIMARY KEY AUTOINCREMENT NOT NULL,[Name] VARCHAR(30)  UNIQUE NOT NULL,[Location] VARCHAR(150)  UNIQUE NOT NULL,[Flags] VARCHAR(3)  NOT NULL,[Staff] INTEGER DEFAULT '''0''' NOT NULL,[StaffCap] INTEGER DEFAULT '''10''' NOT NULL,[Cost] INTEGER  NOT NULL,[IncomeMin] INTEGER DEFAULT '0' NOT NULL,[IncomeMax] INTEGER DEFAULT '0' NOT NULL,[StaffSal] INTEGER DEFAULT '0' NOT NULL,[StaffPay] INTEGER DEFAULT '0' NOT NULL,[Income] INTEGER DEFAULT '0' NOT NULL,[TypeID] INTEGER  NOT NULL);</t>
+  </si>
+  <si>
+    <t>Min income value for each staff member</t>
+  </si>
+  <si>
+    <t>Max income value for each staff member</t>
+  </si>
+  <si>
+    <t>Salary paid to every staff member before income calculation</t>
+  </si>
+  <si>
+    <t>If player can't met StaffSal * Staff, no income is calculated</t>
+  </si>
+  <si>
+    <t>Up front payment to hire a new staff member</t>
+  </si>
+  <si>
+    <t>Can be 0</t>
+  </si>
+  <si>
+    <t>Income to collect</t>
+  </si>
+  <si>
+    <t>This value is calculated like follows: Random(IncomeMin, IncomeMax) * Staff</t>
+  </si>
+  <si>
+    <t>Calculations run every minute</t>
+  </si>
+  <si>
+    <t>Refer to Types page</t>
+  </si>
+  <si>
+    <t>Stored as a 3 char string</t>
   </si>
 </sst>
 </file>
@@ -202,7 +220,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,14 +258,8 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,8 +278,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -338,21 +356,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -468,7 +471,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -480,13 +483,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -496,51 +514,6 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -575,7 +548,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -603,35 +576,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
@@ -640,13 +607,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -952,14 +919,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="105.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1036,14 +1004,14 @@
       <c r="A10" s="11"/>
       <c r="B10" s="15"/>
       <c r="C10" s="12" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="15"/>
       <c r="C11" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1059,7 +1027,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1085,7 +1053,7 @@
         <v>24</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1111,14 +1079,14 @@
         <v>25</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="15"/>
       <c r="C22" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1136,18 +1104,16 @@
         <v>27</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="15"/>
-      <c r="C26" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="C26" s="12"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
@@ -1159,8 +1125,145 @@
       <c r="B28" s="24"/>
       <c r="C28" s="14"/>
     </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="12"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="12"/>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="13"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="14"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="12"/>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="13"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="14"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="12"/>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="13"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="14"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="11"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="13"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="14"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="11"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="12"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="11"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="12"/>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="13"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="14"/>
+    </row>
   </sheetData>
-  <sheetProtection password="85FC" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1168,165 +1271,172 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" style="25" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" style="25" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" style="25" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="25"/>
+    <col min="3" max="3" width="10.140625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="13" style="25" customWidth="1"/>
+    <col min="5" max="5" width="49" style="25" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="25" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="30" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="32">
-        <v>0</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="32">
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="28">
         <v>1</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B2" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="32"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="28">
+        <v>2</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="32"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="28">
+        <v>3</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="32"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="28">
+        <v>4</v>
+      </c>
+      <c r="B5" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="32">
-        <v>2</v>
-      </c>
-      <c r="B4" s="28" t="s">
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="32"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="28">
+        <v>5</v>
+      </c>
+      <c r="B6" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="32">
-        <v>3</v>
-      </c>
-      <c r="B5" s="28" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="32"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="28">
+        <v>6</v>
+      </c>
+      <c r="B7" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="32">
-        <v>4</v>
-      </c>
-      <c r="B6" s="28" t="s">
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="32"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="28">
+        <v>7</v>
+      </c>
+      <c r="B8" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="32">
-        <v>5</v>
-      </c>
-      <c r="B7" s="28" t="s">
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="32"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="28">
+        <v>8</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="32"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="28">
+        <v>9</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="32"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="30">
+        <v>10</v>
+      </c>
+      <c r="B11" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="32">
-        <v>6</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="32">
-        <v>7</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="32">
-        <v>8</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="32">
-        <v>9</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="34">
-        <v>10</v>
-      </c>
-      <c r="B12" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>53</v>
-      </c>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="32"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
     </row>
   </sheetData>
-  <sheetProtection password="85FC" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomLeft" activeCell="M11" sqref="M2:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,12 +1445,13 @@
     <col min="2" max="2" width="29" style="5" customWidth="1"/>
     <col min="3" max="5" width="9.140625" style="5"/>
     <col min="6" max="6" width="13.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="5"/>
-    <col min="8" max="8" width="100.7109375" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="11" width="13.85546875" style="8" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="5"/>
+    <col min="13" max="13" width="100.7109375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
@@ -1359,14 +1470,29 @@
       <c r="F1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M1" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1385,15 +1511,30 @@
       <c r="F2" s="7">
         <v>599999</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="7">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7">
+        <v>0</v>
+      </c>
+      <c r="I2" s="7">
+        <v>0</v>
+      </c>
+      <c r="J2" s="7">
+        <v>0</v>
+      </c>
+      <c r="K2" s="7">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="str">
-        <f>"INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('" &amp;A2&amp;"','" &amp;B2&amp; "','"&amp;C2&amp;"',"&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;G2&amp;");"</f>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('Grotti','79.76576,801.2764,15.16314','101',0,10,599999,1);</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M2" s="1" t="str">
+        <f>"INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('" &amp;A2&amp;"','" &amp;B2&amp; "','"&amp;C2&amp;"',"&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;G2&amp;", "&amp;H2&amp;", "&amp;I2&amp;", "&amp;J2&amp;", "&amp;K2&amp;","&amp;L2&amp;");"</f>
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Grotti','79.76576,801.2764,15.16314','101',0,10,599999,0, 0, 0, 0, 0,1);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -1412,15 +1553,30 @@
       <c r="F3" s="7">
         <v>399999</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4">
         <v>2</v>
       </c>
-      <c r="H3" s="1" t="str">
-        <f t="shared" ref="H3:H11" si="0">"INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('" &amp;A3&amp;"','" &amp;B3&amp; "','"&amp;C3&amp;"',"&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;");"</f>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('Perseus','22.08282,805.9178,14.76683','100',0,10,399999,2);</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M3" s="1" t="str">
+        <f t="shared" ref="M3:M11" si="0">"INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('" &amp;A3&amp;"','" &amp;B3&amp; "','"&amp;C3&amp;"',"&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;", "&amp;H3&amp;", "&amp;I3&amp;", "&amp;J3&amp;", "&amp;K3&amp;","&amp;L3&amp;");"</f>
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Perseus','22.08282,805.9178,14.76683','100',0,10,399999,0, 0, 0, 0, 0,2);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -1439,15 +1595,30 @@
       <c r="F4" s="7">
         <v>10000</v>
       </c>
-      <c r="G4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1" t="str">
+      <c r="G4" s="7">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0</v>
+      </c>
+      <c r="K4" s="7">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('Shodi','14.46907,944.1911,14.71485','100',0,10,10000,0);</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Shodi','14.46907,944.1911,14.71485','100',0,10,10000,0, 0, 0, 0, 0,0);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1466,15 +1637,30 @@
       <c r="F5" s="7">
         <v>100000</v>
       </c>
-      <c r="G5" s="4">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1" t="str">
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('SuperStar','18.07519,980.3729,15.64596','101',0,10,100000,0);</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('SuperStar','18.07519,980.3729,15.64596','101',0,10,100000,0, 0, 0, 0, 0,0);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -1493,15 +1679,30 @@
       <c r="F6" s="7">
         <v>250000</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0</v>
+      </c>
+      <c r="K6" s="7">
+        <v>0</v>
+      </c>
+      <c r="L6" s="4">
         <v>5</v>
       </c>
-      <c r="H6" s="1" t="str">
+      <c r="M6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('Apartment Block','66.77424,968.6838,13.65716','100',0,50,250000,5);</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Apartment Block','66.77424,968.6838,13.65716','100',0,50,250000,0, 0, 0, 0, 0,5);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -1520,15 +1721,30 @@
       <c r="F7" s="7">
         <v>100000</v>
       </c>
-      <c r="G7" s="4">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1" t="str">
+      <c r="G7" s="7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="7">
+        <v>0</v>
+      </c>
+      <c r="K7" s="7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('TerrOil','105.8526,1120.935,14.67003','100',0,10,100000,0);</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('TerrOil','105.8526,1120.935,14.67003','100',0,10,100000,0, 0, 0, 0, 0,0);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -1547,15 +1763,30 @@
       <c r="F8" s="7">
         <v>1000000</v>
       </c>
-      <c r="G8" s="4">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1" t="str">
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7">
+        <v>0</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('Liberty City Delivery','-24.0677,880.597,18.74995','100',0,100,1000000,0);</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Liberty City Delivery','-24.0677,880.597,18.74995','100',0,100,1000000,0, 0, 0, 0, 0,0);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1574,15 +1805,30 @@
       <c r="F9" s="7">
         <v>15000000</v>
       </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1" t="str">
+      <c r="G9" s="7">
+        <v>0</v>
+      </c>
+      <c r="H9" s="7">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0</v>
+      </c>
+      <c r="K9" s="7">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('The Libertonian Museum','-86.32443,821.8265,18.63036','100',0,50,15000000,0);</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('The Libertonian Museum','-86.32443,821.8265,18.63036','100',0,50,15000000,0, 0, 0, 0, 0,0);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1601,15 +1847,30 @@
       <c r="F10" s="7">
         <v>250000</v>
       </c>
-      <c r="G10" s="4">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1" t="str">
+      <c r="G10" s="7">
+        <v>0</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7">
+        <v>0</v>
+      </c>
+      <c r="J10" s="7">
+        <v>0</v>
+      </c>
+      <c r="K10" s="7">
+        <v>0</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('Office Block','25.91283,589.9072,14.71847','100',0,100,250000,0);</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Office Block','25.91283,589.9072,14.71847','100',0,100,250000,0, 0, 0, 0, 0,0);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1628,12 +1889,27 @@
       <c r="F11" s="7">
         <v>100000</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="7">
+        <v>0</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7">
+        <v>0</v>
+      </c>
+      <c r="J11" s="7">
+        <v>0</v>
+      </c>
+      <c r="K11" s="7">
+        <v>0</v>
+      </c>
+      <c r="L11" s="4">
         <v>10</v>
       </c>
-      <c r="H11" s="1" t="str">
+      <c r="M11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('Construction Site','72.04861,612.6984,14.71273','100',0,50,100000,10);</v>
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Construction Site','72.04861,612.6984,14.71273','100',0,50,100000,0, 0, 0, 0, 0,10);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>